<commit_message>
more of cp6 done
</commit_message>
<xml_diff>
--- a/lab_reports/viscosity_of_water/viscosity_of_water.xlsx
+++ b/lab_reports/viscosity_of_water/viscosity_of_water.xlsx
@@ -12,12 +12,12 @@
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680"/>
   </bookViews>
   <sheets>
-    <sheet name="Jon's " sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'Jon''s '!$T$38</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Data!$T$38</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -32,7 +32,7 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'Jon''s '!$T$36</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Data!$T$36</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
@@ -1152,7 +1152,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1197,8 +1197,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1479,9 +1483,6 @@
     <xf numFmtId="1" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1497,8 +1498,14 @@
     <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="48">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1521,6 +1528,8 @@
     <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1542,6 +1551,8 @@
     <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1614,7 +1625,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Jon''s '!$E$4:$E$16</c:f>
+                <c:f>Data!$E$4:$E$16</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="13"/>
@@ -1662,7 +1673,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Jon''s '!$E$4:$E$16</c:f>
+                <c:f>Data!$E$4:$E$16</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="13"/>
@@ -1711,7 +1722,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'Jon''s '!$B$4:$B$16</c:f>
+              <c:f>Data!$B$4:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1759,7 +1770,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Jon''s '!$D$4:$D$16</c:f>
+              <c:f>Data!$D$4:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1840,7 +1851,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Jon''s '!$B$20:$B$35</c:f>
+              <c:f>Data!$B$20:$B$35</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1888,7 +1899,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Jon''s '!$C$20:$C$35</c:f>
+              <c:f>Data!$C$20:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="16"/>
@@ -1961,7 +1972,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Jon''s '!$K$4:$K$16</c:f>
+              <c:f>Data!$K$4:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1994,7 +2005,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Jon''s '!$M$4:$M$16</c:f>
+              <c:f>Data!$M$4:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2049,7 +2060,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Jon''s '!$T$4:$T$16</c:f>
+              <c:f>Data!$T$4:$T$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2082,7 +2093,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Jon''s '!$V$4:$V$16</c:f>
+              <c:f>Data!$V$4:$V$16</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2143,7 +2154,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Jon''s '!$I$20:$I$35</c:f>
+              <c:f>Data!$I$20:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2176,7 +2187,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Jon''s '!$J$20:$J$35</c:f>
+              <c:f>Data!$J$20:$J$35</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2237,7 +2248,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Jon''s '!$P$20:$P$35</c:f>
+              <c:f>Data!$P$20:$P$35</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2270,7 +2281,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Jon''s '!$Q$20:$Q$35</c:f>
+              <c:f>Data!$Q$20:$Q$35</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2393,6 +2404,2781 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>blue</a:t>
+            </a:r>
+            <a:endParaRPr lang="el-GR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$C$60</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>μ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$B$61:$B$73</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$C$61:$C$73</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>-0.00361916191487616</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00901570157213022</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.00612721271864121</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.0123812381205237</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.0230797079668507</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0106662666312668</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00330113011827315</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.00961956195027605</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.0314291429077141</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.0165720571984855</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0127294729551875</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0291103110403114</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0432689269032129</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-986942304"/>
+        <c:axId val="-1006689376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-986942304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1006689376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1006689376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-986942304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>red</a:t>
+            </a:r>
+            <a:endParaRPr lang="el-GR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$G$60</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>μ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$F$61:$F$68</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$G$61:$G$68</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-0.000742944368045364</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00129188904168705</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.0200066108819139</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0036948891944852</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.00927027739578238</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.0100132217638277</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00313272275701579</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0251675561667482</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-987042480"/>
+        <c:axId val="-987044800"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-987042480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-987044800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-987044800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-987042480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>black</a:t>
+            </a:r>
+            <a:endParaRPr lang="el-GR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$K$60</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>μ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$J$61:$J$68</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$K$61:$K$68</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-0.00152811867461863</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00583265153965163</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.00791768935718921</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.00611247469847452</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.000973926706426472</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00527573239673269</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00985872483322515</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.0100027271747268</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1010039408"/>
+        <c:axId val="-1010376976"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1010039408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1010376976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1010376976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1010039408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2699,6 +5485,96 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>302026</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>149198</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>647807</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>131270</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>170542</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>519740</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>32229</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>632867</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>149199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>284951</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>10887</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2991,8 +5867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="O44" sqref="O44"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="119" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="K93" sqref="K93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6094,7 +8970,7 @@
       <c r="S57" s="1"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B59" s="98" t="s">
+      <c r="B59" s="97" t="s">
         <v>41</v>
       </c>
       <c r="G59" s="86"/>
@@ -6105,32 +8981,32 @@
       <c r="L59" s="88"/>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A60" s="98" t="s">
+      <c r="A60" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="B60" s="96" t="s">
+      <c r="B60" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="C60" s="97" t="s">
+      <c r="C60" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="E60" s="98" t="s">
+      <c r="E60" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="F60" s="93" t="s">
+      <c r="F60" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="G60" s="94" t="s">
+      <c r="G60" s="96" t="s">
         <v>26</v>
       </c>
       <c r="H60" s="87"/>
-      <c r="I60" s="99" t="s">
+      <c r="I60" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="J60" s="93" t="s">
+      <c r="J60" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="K60" s="94" t="s">
+      <c r="K60" s="96" t="s">
         <v>26</v>
       </c>
       <c r="L60" s="90"/>
@@ -6139,21 +9015,21 @@
       <c r="B61" s="93">
         <v>2</v>
       </c>
-      <c r="C61" s="95">
+      <c r="C61" s="94">
         <v>-3.6191619148761567E-3</v>
       </c>
       <c r="F61" s="93">
         <v>2</v>
       </c>
-      <c r="G61" s="95">
+      <c r="G61" s="94">
         <v>-7.4294436804536387E-4</v>
       </c>
       <c r="H61" s="87"/>
       <c r="I61" s="89"/>
-      <c r="J61" s="93">
+      <c r="J61" s="99">
         <v>2</v>
       </c>
-      <c r="K61" s="95">
+      <c r="K61" s="100">
         <v>-1.5281186746186302E-3</v>
       </c>
       <c r="L61" s="90"/>
@@ -6162,13 +9038,13 @@
       <c r="B62" s="93">
         <v>3</v>
       </c>
-      <c r="C62" s="95">
+      <c r="C62" s="94">
         <v>9.0157015721302192E-3</v>
       </c>
       <c r="F62" s="93">
         <v>4</v>
       </c>
-      <c r="G62" s="95">
+      <c r="G62" s="94">
         <v>1.2918890416870471E-3</v>
       </c>
       <c r="H62" s="87"/>
@@ -6176,7 +9052,7 @@
       <c r="J62" s="93">
         <v>4</v>
       </c>
-      <c r="K62" s="95">
+      <c r="K62" s="94">
         <v>5.8326515396516267E-3</v>
       </c>
       <c r="L62" s="90"/>
@@ -6185,21 +9061,21 @@
       <c r="B63" s="93">
         <v>4</v>
       </c>
-      <c r="C63" s="95">
+      <c r="C63" s="94">
         <v>-6.127212718641209E-3</v>
       </c>
       <c r="F63" s="93">
-        <v>8</v>
-      </c>
-      <c r="G63" s="95">
-        <v>3.6948891944851986E-3</v>
+        <v>6</v>
+      </c>
+      <c r="G63" s="94">
+        <v>-2.0006610881913862E-2</v>
       </c>
       <c r="H63" s="87"/>
       <c r="I63" s="89"/>
       <c r="J63" s="93">
         <v>6</v>
       </c>
-      <c r="K63" s="95">
+      <c r="K63" s="94">
         <v>-7.9176893571892143E-3</v>
       </c>
       <c r="L63" s="90"/>
@@ -6208,21 +9084,21 @@
       <c r="B64" s="93">
         <v>5</v>
       </c>
-      <c r="C64" s="95">
+      <c r="C64" s="94">
         <v>-1.2381238120523733E-2</v>
       </c>
       <c r="F64" s="93">
-        <v>10</v>
-      </c>
-      <c r="G64" s="95">
-        <v>-9.2702773957823864E-3</v>
+        <v>8</v>
+      </c>
+      <c r="G64" s="94">
+        <v>3.6948891944851986E-3</v>
       </c>
       <c r="H64" s="87"/>
       <c r="I64" s="89"/>
       <c r="J64" s="93">
         <v>8</v>
       </c>
-      <c r="K64" s="95">
+      <c r="K64" s="94">
         <v>-6.112474698474521E-3</v>
       </c>
       <c r="L64" s="90"/>
@@ -6231,21 +9107,21 @@
       <c r="B65" s="93">
         <v>6</v>
       </c>
-      <c r="C65" s="95">
+      <c r="C65" s="94">
         <v>-2.3079707966850674E-2</v>
       </c>
       <c r="F65" s="93">
-        <v>12</v>
-      </c>
-      <c r="G65" s="95">
-        <v>-1.0013221763827712E-2</v>
+        <v>10</v>
+      </c>
+      <c r="G65" s="94">
+        <v>-9.2702773957823864E-3</v>
       </c>
       <c r="H65" s="87"/>
       <c r="I65" s="89"/>
       <c r="J65" s="93">
         <v>10</v>
       </c>
-      <c r="K65" s="95">
+      <c r="K65" s="94">
         <v>-9.7392670642647283E-4</v>
       </c>
       <c r="L65" s="90"/>
@@ -6254,21 +9130,21 @@
       <c r="B66" s="93">
         <v>7</v>
       </c>
-      <c r="C66" s="95">
+      <c r="C66" s="94">
         <v>1.0666266631266824E-2</v>
       </c>
       <c r="F66" s="93">
-        <v>14</v>
-      </c>
-      <c r="G66" s="95">
-        <v>3.1327227570157878E-3</v>
+        <v>12</v>
+      </c>
+      <c r="G66" s="94">
+        <v>-1.0013221763827712E-2</v>
       </c>
       <c r="H66" s="87"/>
       <c r="I66" s="89"/>
       <c r="J66" s="93">
         <v>12</v>
       </c>
-      <c r="K66" s="95">
+      <c r="K66" s="94">
         <v>5.2757323967326936E-3</v>
       </c>
       <c r="L66" s="90"/>
@@ -6277,21 +9153,21 @@
       <c r="B67" s="93">
         <v>8</v>
       </c>
-      <c r="C67" s="95">
+      <c r="C67" s="94">
         <v>3.3011301182731545E-3</v>
       </c>
       <c r="F67" s="93">
-        <v>16</v>
-      </c>
-      <c r="G67" s="95">
-        <v>2.5167556166748206E-2</v>
+        <v>14</v>
+      </c>
+      <c r="G67" s="94">
+        <v>3.1327227570157878E-3</v>
       </c>
       <c r="H67" s="87"/>
       <c r="I67" s="89"/>
       <c r="J67" s="93">
         <v>14</v>
       </c>
-      <c r="K67" s="95">
+      <c r="K67" s="94">
         <v>9.8587248332251548E-3</v>
       </c>
       <c r="L67" s="90"/>
@@ -6300,17 +9176,21 @@
       <c r="B68" s="93">
         <v>9</v>
       </c>
-      <c r="C68" s="95">
+      <c r="C68" s="94">
         <v>-9.619561950276051E-3</v>
       </c>
-      <c r="F68" s="87"/>
-      <c r="G68" s="89"/>
+      <c r="F68" s="93">
+        <v>16</v>
+      </c>
+      <c r="G68" s="94">
+        <v>2.5167556166748206E-2</v>
+      </c>
       <c r="H68" s="87"/>
       <c r="I68" s="89"/>
       <c r="J68" s="93">
         <v>16</v>
       </c>
-      <c r="K68" s="95">
+      <c r="K68" s="94">
         <v>-1.0002727174726833E-2</v>
       </c>
       <c r="L68" s="90"/>
@@ -6319,7 +9199,7 @@
       <c r="B69" s="93">
         <v>10</v>
       </c>
-      <c r="C69" s="95">
+      <c r="C69" s="94">
         <v>-3.1429142907714119E-2</v>
       </c>
       <c r="F69" s="87"/>
@@ -6334,7 +9214,7 @@
       <c r="B70" s="93">
         <v>11</v>
       </c>
-      <c r="C70" s="95">
+      <c r="C70" s="94">
         <v>-1.6572057198485507E-2</v>
       </c>
       <c r="F70" s="87"/>
@@ -6349,7 +9229,7 @@
       <c r="B71" s="93">
         <v>12</v>
       </c>
-      <c r="C71" s="95">
+      <c r="C71" s="94">
         <v>1.2729472955187504E-2</v>
       </c>
       <c r="F71" s="87"/>
@@ -6364,7 +9244,7 @@
       <c r="B72" s="93">
         <v>14</v>
       </c>
-      <c r="C72" s="95">
+      <c r="C72" s="94">
         <v>2.9110311040311421E-2</v>
       </c>
       <c r="F72" s="87"/>
@@ -6379,7 +9259,7 @@
       <c r="B73" s="93">
         <v>16</v>
       </c>
-      <c r="C73" s="95">
+      <c r="C73" s="94">
         <v>4.3268926903212934E-2</v>
       </c>
       <c r="F73" s="87"/>

</xml_diff>